<commit_message>
Added API Testing and Cucumber
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,42 +19,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
-  <si>
-    <t>TestOne</t>
-  </si>
-  <si>
-    <t>TestTwo</t>
-  </si>
-  <si>
-    <t>TestThree</t>
-  </si>
-  <si>
-    <t>TestFour</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+  <si>
+    <t>catdog</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
   <si>
     <t>UserName</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>PassOne</t>
-  </si>
-  <si>
-    <t>PassTwo</t>
-  </si>
-  <si>
-    <t>PassFour</t>
+    <t>dogcat</t>
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>PassThree</t>
   </si>
 </sst>
 </file>
@@ -403,26 +385,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="190" zoomScaleNormal="190">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -430,43 +410,43 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>